<commit_message>
initialize class preprocessing from the instance, end fixing the authlog table, many fixes necesary
</commit_message>
<xml_diff>
--- a/data_dictionary/Diccionario_FBS.xlsx
+++ b/data_dictionary/Diccionario_FBS.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="creditos" sheetId="1" r:id="rId1"/>
+    <sheet name="radicados" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="130">
   <si>
     <t>Dias Mora Actual</t>
   </si>
@@ -321,19 +322,118 @@
   </si>
   <si>
     <t>tiempo_de_espera</t>
+  </si>
+  <si>
+    <t>Tiempo en dias desde la solicitud de credito hasta el desembolso</t>
+  </si>
+  <si>
+    <t>Tiempo en dias desde la solicitud realizada hasta el inicio del proceso</t>
+  </si>
+  <si>
+    <t>Tiempo en dias desde la solicitud de credito hasta la legalización del mismo</t>
+  </si>
+  <si>
+    <t>Fecha del momento del analisis de la información</t>
+  </si>
+  <si>
+    <t>Tiempo en dias desde la solicitud hasta la fecha actual</t>
+  </si>
+  <si>
+    <t>Radicado</t>
+  </si>
+  <si>
+    <t>Fecha Radicacion</t>
+  </si>
+  <si>
+    <t>Procedencia</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Naturaleza</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>Expediente</t>
+  </si>
+  <si>
+    <t>Rpta</t>
+  </si>
+  <si>
+    <t>Opciones</t>
+  </si>
+  <si>
+    <t>cargo_destino</t>
+  </si>
+  <si>
+    <t>cod_grupo_destino</t>
+  </si>
+  <si>
+    <t>funcionario_destino</t>
+  </si>
+  <si>
+    <t>grupo_destino</t>
+  </si>
+  <si>
+    <t>Id del radicado</t>
+  </si>
+  <si>
+    <t>Alfanet</t>
+  </si>
+  <si>
+    <t>Fecha en la cual fue radicada la solicitud</t>
+  </si>
+  <si>
+    <t>Funcionario que realiza la peticion o el trámite</t>
+  </si>
+  <si>
+    <t>Asunto de la solicitud radicada por el usuario</t>
+  </si>
+  <si>
+    <t>Etiqueta que califica los radicados para entendimiento del equipo</t>
+  </si>
+  <si>
+    <t>Canal utilizado para realizar la solcitud</t>
+  </si>
+  <si>
+    <t>Funcionario o grupo al que se designa la solicitud</t>
+  </si>
+  <si>
+    <t>Valor que denota si ya se ha dado respuesta o no a la solicitud inicial. 0=no hay respuesta, 1=si hubo respuesta.</t>
+  </si>
+  <si>
+    <t>Cargo del funcionario designado para dar respuesta</t>
+  </si>
+  <si>
+    <t>Código del grupo designado para dar respuesta</t>
+  </si>
+  <si>
+    <t>Nombre completo del funcionario designado para dar respuesta</t>
+  </si>
+  <si>
+    <t>Nombre del grupo designado para dar respuesta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,7 +444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -352,13 +452,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -643,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,6 +1521,15 @@
       <c r="B44" t="s">
         <v>42</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1411,13 +1538,31 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
       <c r="B46" t="s">
         <v>42</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,6 +1572,15 @@
       <c r="B47" t="s">
         <v>50</v>
       </c>
+      <c r="C47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1434,6 +1588,295 @@
       </c>
       <c r="B48" t="s">
         <v>42</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last changes, adjustments in column formats between modeled and raw extraction.
</commit_message>
<xml_diff>
--- a/data_dictionary/Diccionario_FBS.xlsx
+++ b/data_dictionary/Diccionario_FBS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="creditos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="131">
   <si>
     <t>Dias Mora Actual</t>
   </si>
@@ -415,13 +415,16 @@
   </si>
   <si>
     <t>Nombre del grupo designado para dar respuesta</t>
+  </si>
+  <si>
+    <t>Sujeto_auditoria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +437,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -471,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -479,6 +490,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,19 +772,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -790,8 +804,11 @@
       <c r="F1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -807,8 +824,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -827,8 +847,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -844,13 +867,16 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>47</v>
@@ -861,13 +887,16 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
+      <c r="B6" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>48</v>
@@ -878,8 +907,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -895,8 +927,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -912,8 +947,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -929,8 +967,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -946,8 +987,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -963,8 +1007,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -980,8 +1027,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -997,8 +1047,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1014,13 +1067,16 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>61</v>
@@ -1031,8 +1087,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1051,8 +1110,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1068,8 +1130,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1085,8 +1150,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1102,8 +1170,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1119,8 +1190,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1136,8 +1210,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1156,8 +1233,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1173,12 +1253,15 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1190,8 +1273,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1207,13 +1293,16 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>72</v>
@@ -1224,8 +1313,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1241,8 +1333,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1258,8 +1353,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1275,8 +1373,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1292,8 +1393,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1309,8 +1413,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1326,8 +1433,11 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1343,8 +1453,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1360,8 +1473,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1377,8 +1493,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1394,8 +1513,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1411,8 +1533,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1428,8 +1553,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1445,8 +1573,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1462,8 +1593,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -1479,8 +1613,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -1496,8 +1633,11 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1513,8 +1653,11 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -1530,8 +1673,11 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -1547,12 +1693,15 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1564,8 +1713,11 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1581,8 +1733,11 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1597,6 +1752,9 @@
       </c>
       <c r="F48">
         <v>1</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1607,19 +1765,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1638,8 +1797,11 @@
       <c r="F1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>104</v>
       </c>
@@ -1658,8 +1820,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
@@ -1675,8 +1840,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>106</v>
       </c>
@@ -1695,8 +1863,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>107</v>
       </c>
@@ -1712,8 +1883,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>108</v>
       </c>
@@ -1729,8 +1903,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
@@ -1746,8 +1923,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>110</v>
       </c>
@@ -1761,8 +1941,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1778,8 +1961,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>111</v>
       </c>
@@ -1795,8 +1981,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>112</v>
       </c>
@@ -1810,8 +1999,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>113</v>
       </c>
@@ -1827,8 +2019,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>114</v>
       </c>
@@ -1844,8 +2039,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>115</v>
       </c>
@@ -1861,8 +2059,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>116</v>
       </c>
@@ -1877,6 +2078,9 @@
       </c>
       <c r="F15">
         <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>